<commit_message>
fixed bug on customer feedback excel file
</commit_message>
<xml_diff>
--- a/quality/src/main/resources/customer_feedback_form.xlsx
+++ b/quality/src/main/resources/customer_feedback_form.xlsx
@@ -250,13 +250,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Wingdings"/>
-      <family val="0"/>
-      <charset val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -265,10 +258,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Wingdings"/>
-      <family val="0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -284,6 +277,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings"/>
+      <family val="0"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -349,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,15 +394,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,27 +430,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,15 +446,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,8 +473,8 @@
   </sheetPr>
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,212 +716,251 @@
       <c r="K18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S18" s="16" t="s">
+      <c r="Q18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S18" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="16"/>
+      <c r="Q19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S20" s="16" t="s">
+      <c r="Q20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S20" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="M22" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S22" s="16" t="s">
+      <c r="Q22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S22" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="Q23" s="16"/>
+    </row>
+    <row r="24" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="15" t="s">
+      <c r="M24" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O24" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q24" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S24" s="16" t="s">
+      <c r="Q24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S24" s="15" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="Q25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M26" s="15" t="s">
+      <c r="M26" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="16" t="s">
+      <c r="Q26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S26" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="Q27" s="16"/>
+    </row>
     <row r="28" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M28" s="15" t="s">
+      <c r="M28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O28" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="16" t="s">
+      <c r="Q28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S28" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="Q29" s="16"/>
+    </row>
     <row r="30" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M30" s="15" t="s">
+      <c r="M30" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O30" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S30" s="16" t="s">
+      <c r="Q30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S30" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="Q31" s="16"/>
+    </row>
     <row r="32" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M32" s="15" t="s">
+      <c r="M32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O32" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q32" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S32" s="16" t="s">
+      <c r="Q32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S32" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="Q33" s="16"/>
+    </row>
+    <row r="34" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="13" t="s">
         <v>16</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M34" s="15" t="s">
+      <c r="M34" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O34" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q34" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S34" s="16" t="s">
+      <c r="Q34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S34" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="16"/>
+      <c r="M35" s="16"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J36" s="1" t="s">
@@ -934,7 +969,7 @@
       <c r="K36" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="M36" s="15" t="s">
+      <c r="M36" s="13" t="s">
         <v>16</v>
       </c>
       <c r="O36" s="19" t="s">
@@ -942,11 +977,11 @@
       </c>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="20"/>
+      <c r="M37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="18"/>
@@ -1114,7 +1149,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1223,7 +1258,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
@@ -1251,9 +1286,9 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>43</v>
       </c>
       <c r="R11" s="7" t="s">
@@ -1263,13 +1298,13 @@
     </row>
     <row r="12" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="26"/>
+      <c r="D12" s="25"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
         <v>16</v>
       </c>
@@ -1296,11 +1331,10 @@
       </c>
     </row>
     <row r="14" s="5" customFormat="true" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="25"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
@@ -1324,14 +1358,13 @@
       </c>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="25"/>
+    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
@@ -1351,14 +1384,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="25"/>
+    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1409,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
@@ -1397,7 +1429,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>